<commit_message>
Cleaning up function code
</commit_message>
<xml_diff>
--- a/inst/extdata/bball-examples.xlsx
+++ b/inst/extdata/bball-examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Data\r-projects\unpivotr-dev\unpivotr\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianmo\OneDrive\Documents\data\projects\unpivotr-dev\unpivotr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42363886-0E25-4423-B75F-944FE28E4112}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D27209-408F-4647-81B7-2CE049E1E3D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{8F000A3E-8BE5-41FF-9439-0142BAC800EC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{8F000A3E-8BE5-41FF-9439-0142BAC800EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,16 +242,10 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,6 +265,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,7 +589,7 @@
   <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,467 +598,467 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>6</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>17</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>0.35299999999999998</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>14</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>11</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>15</v>
       </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-      <c r="J6" s="12">
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>12</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>0.33300000000000002</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>10</v>
       </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12">
-        <v>3</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>7</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>8</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>0.875</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>14</v>
       </c>
-      <c r="F8" s="12">
-        <v>3</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="F8" s="10">
+        <v>3</v>
+      </c>
+      <c r="G8" s="10">
         <v>6</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>9</v>
       </c>
-      <c r="I8" s="12">
-        <v>2</v>
-      </c>
-      <c r="J8" s="12">
+      <c r="I8" s="10">
+        <v>2</v>
+      </c>
+      <c r="J8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>13</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>0.46200000000000002</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>17</v>
       </c>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12">
-        <v>2</v>
-      </c>
-      <c r="I9" s="12">
-        <v>0</v>
-      </c>
-      <c r="J9" s="12">
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <v>18</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0.27800000000000002</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>16</v>
       </c>
-      <c r="F10" s="12">
-        <v>2</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10">
         <v>6</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>35</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>89</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>0.39300000000000002</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>95</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>13</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <v>34</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>47</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <v>5</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>16</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="10">
         <v>23</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>45</v>
       </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
         <v>11</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <v>11</v>
       </c>
-      <c r="I13" s="12">
-        <v>2</v>
-      </c>
-      <c r="J13" s="12">
+      <c r="I13" s="10">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>4</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="10">
         <v>10</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>0.4</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>9</v>
       </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="12">
-        <v>2</v>
-      </c>
-      <c r="H14" s="12">
-        <v>3</v>
-      </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="12">
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <v>15</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <v>0.8</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>29</v>
       </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
         <v>7</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>7</v>
       </c>
-      <c r="I15" s="12">
-        <v>0</v>
-      </c>
-      <c r="J15" s="12">
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10">
         <v>5</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <v>0.4</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>7</v>
       </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
-        <v>3</v>
-      </c>
-      <c r="H16" s="12">
-        <v>3</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3</v>
+      </c>
+      <c r="H16" s="10">
+        <v>3</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="12">
-        <v>3</v>
-      </c>
-      <c r="C17" s="12">
+      <c r="B17" s="10">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10">
         <v>8</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <v>0.375</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>8</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
-        <v>2</v>
-      </c>
-      <c r="H17" s="12">
-        <v>2</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <v>41</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="10">
         <v>79</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="10">
         <v>0.51900000000000002</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="10">
         <v>108</v>
       </c>
-      <c r="F18" s="12">
-        <v>2</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="F18" s="10">
+        <v>2</v>
+      </c>
+      <c r="G18" s="10">
         <v>38</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>40</v>
       </c>
-      <c r="I18" s="12">
-        <v>3</v>
-      </c>
-      <c r="J18" s="12">
+      <c r="I18" s="10">
+        <v>3</v>
+      </c>
+      <c r="J18" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1087,467 +1087,467 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>1</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="A6" s="12">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10">
         <v>6</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>17</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>0.35299999999999998</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>14</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>11</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>15</v>
       </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-      <c r="J6" s="12">
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="12">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>12</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>0.33300000000000002</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>10</v>
       </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12">
-        <v>3</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>3</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" s="12">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10">
         <v>7</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>8</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>0.875</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>14</v>
       </c>
-      <c r="F8" s="12">
-        <v>3</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="F8" s="10">
+        <v>3</v>
+      </c>
+      <c r="G8" s="10">
         <v>6</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>9</v>
       </c>
-      <c r="I8" s="12">
-        <v>2</v>
-      </c>
-      <c r="J8" s="12">
+      <c r="I8" s="10">
+        <v>2</v>
+      </c>
+      <c r="J8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="12">
         <v>4</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>13</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>0.46200000000000002</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>17</v>
       </c>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12">
-        <v>2</v>
-      </c>
-      <c r="I9" s="12">
-        <v>0</v>
-      </c>
-      <c r="J9" s="12">
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="12">
         <v>5</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <v>18</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0.27800000000000002</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>16</v>
       </c>
-      <c r="F10" s="12">
-        <v>2</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10">
         <v>6</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>35</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>89</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>0.39300000000000002</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>95</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>13</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <v>34</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>47</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <v>5</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12">
+      <c r="A13" s="12">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10">
         <v>16</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="10">
         <v>23</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>45</v>
       </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
         <v>11</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <v>11</v>
       </c>
-      <c r="I13" s="12">
-        <v>2</v>
-      </c>
-      <c r="J13" s="12">
+      <c r="I13" s="10">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12">
+      <c r="A14" s="12">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10">
         <v>4</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="10">
         <v>10</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>0.4</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>9</v>
       </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="12">
-        <v>2</v>
-      </c>
-      <c r="H14" s="12">
-        <v>3</v>
-      </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="12">
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>3</v>
-      </c>
-      <c r="B15" s="12">
+      <c r="A15" s="12">
+        <v>3</v>
+      </c>
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <v>15</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <v>0.8</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>29</v>
       </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
         <v>7</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>7</v>
       </c>
-      <c r="I15" s="12">
-        <v>0</v>
-      </c>
-      <c r="J15" s="12">
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="12">
         <v>4</v>
       </c>
-      <c r="B16" s="12">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10">
         <v>5</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <v>0.4</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>7</v>
       </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
-        <v>3</v>
-      </c>
-      <c r="H16" s="12">
-        <v>3</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3</v>
+      </c>
+      <c r="H16" s="10">
+        <v>3</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="12">
         <v>5</v>
       </c>
-      <c r="B17" s="12">
-        <v>3</v>
-      </c>
-      <c r="C17" s="12">
+      <c r="B17" s="10">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10">
         <v>8</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <v>0.375</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>8</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
-        <v>2</v>
-      </c>
-      <c r="H17" s="12">
-        <v>2</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <v>41</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="10">
         <v>79</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="10">
         <v>0.51900000000000002</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="10">
         <v>108</v>
       </c>
-      <c r="F18" s="12">
-        <v>2</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="F18" s="10">
+        <v>2</v>
+      </c>
+      <c r="G18" s="10">
         <v>38</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>40</v>
       </c>
-      <c r="I18" s="12">
-        <v>3</v>
-      </c>
-      <c r="J18" s="12">
+      <c r="I18" s="10">
+        <v>3</v>
+      </c>
+      <c r="J18" s="10">
         <v>6</v>
       </c>
     </row>

</xml_diff>